<commit_message>
added name for Saitoria Saroni
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -3805,7 +3805,7 @@
       <selection pane="topLeft" activeCell="C107" activeCellId="0" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.87"/>
@@ -8627,7 +8627,7 @@
       <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.5"/>
@@ -12360,11 +12360,11 @@
   </sheetPr>
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J123" activeCellId="0" sqref="J123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
@@ -12372,7 +12372,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="29.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="30.26"/>
   </cols>
   <sheetData>
@@ -16237,6 +16237,9 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>122</v>
+      </c>
       <c r="B123" s="0" t="s">
         <v>928</v>
       </c>

</xml_diff>